<commit_message>
respond to query string
</commit_message>
<xml_diff>
--- a/assets/data/events.xlsx
+++ b/assets/data/events.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elsteinh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atrimblx/Documents/events-page/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$41</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -794,29 +800,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="44.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" customWidth="1"/>
-    <col min="10" max="10" width="36.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="44.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -848,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>93</v>
       </c>
@@ -868,7 +874,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -898,7 +904,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -924,7 +930,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -947,7 +953,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -979,7 +985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>76</v>
       </c>
@@ -1011,7 +1017,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>79</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>78</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>96</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -1173,7 +1179,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -1271,7 +1277,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -1291,7 +1297,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>79</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>94</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1415,7 +1421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>97</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>95</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -1631,7 +1637,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -1680,7 +1686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -1703,7 +1709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>84</v>
       </c>
@@ -1716,7 +1722,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>90</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>92</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>99</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>101</v>
       </c>

</xml_diff>